<commit_message>
clustering: norm distance and test on egg data
</commit_message>
<xml_diff>
--- a/data/egg.xlsx
+++ b/data/egg.xlsx
@@ -2427,7 +2427,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2439,6 +2439,18 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -2603,11 +2615,11 @@
     <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2643,16 +2655,16 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3030,7 +3042,7 @@
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="56.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="58.5">
       <c r="A2" s="9">
         <v>44851.83546296296</v>
       </c>
@@ -3071,7 +3083,7 @@
       <c r="P2" s="13"/>
       <c r="Q2" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="30.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="32.25">
       <c r="A3" s="9">
         <v>44851.947280092594</v>
       </c>
@@ -3147,7 +3159,7 @@
       <c r="P4" s="13"/>
       <c r="Q4" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="30.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="32.25">
       <c r="A5" s="9">
         <v>44853.669907407406</v>
       </c>
@@ -3223,7 +3235,7 @@
       <c r="P6" s="13"/>
       <c r="Q6" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="81">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="84.75">
       <c r="A7" s="9">
         <v>44856.37525462963</v>
       </c>
@@ -3342,7 +3354,7 @@
       <c r="P9" s="13"/>
       <c r="Q9" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="30.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="32.25" customFormat="1" s="1">
       <c r="A10" s="2">
         <v>44850.99701388889</v>
       </c>
@@ -3461,7 +3473,7 @@
       <c r="P12" s="13"/>
       <c r="Q12" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="68.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="71.25">
       <c r="A13" s="9" t="s">
         <v>692</v>
       </c>

</xml_diff>

<commit_message>
clustering: fix min max scaling distance error in update centroid
</commit_message>
<xml_diff>
--- a/data/egg.xlsx
+++ b/data/egg.xlsx
@@ -2427,7 +2427,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2444,12 +2444,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -2618,7 +2612,7 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -3553,7 +3547,7 @@
       <c r="P14" s="13"/>
       <c r="Q14" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="30.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="32.25">
       <c r="A15" s="9">
         <v>44851.387604166666</v>
       </c>
@@ -3592,7 +3586,7 @@
       <c r="P15" s="13"/>
       <c r="Q15" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="43.5">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="45">
       <c r="A16" s="9">
         <v>44851.42435185185</v>
       </c>
@@ -3633,7 +3627,7 @@
       <c r="P16" s="13"/>
       <c r="Q16" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="105.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="111">
       <c r="A17" s="9">
         <v>44851.23446759259</v>
       </c>
@@ -3713,7 +3707,7 @@
       <c r="P18" s="13"/>
       <c r="Q18" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="43.5">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="45">
       <c r="A19" s="9">
         <v>44853.60444444444</v>
       </c>

</xml_diff>